<commit_message>
Mouvement de fichiers et Création d'une DataBase en fichier CSV
Ajouts d'un Mode de Création des Skills en lisant un ficher CSV
</commit_message>
<xml_diff>
--- a/Assets/Resources/SkillsData.xlsx
+++ b/Assets/Resources/SkillsData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Perso\Unity Project\TakTik Ele\Assets\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8D0DF728-9EA8-43A6-8326-80BF72F98D1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0FB53F79-DB19-4356-A292-A43E290ADAAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="573" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,7 @@
     <sheet name="Enum" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="84">
   <si>
     <t>#</t>
   </si>
@@ -67,9 +68,6 @@
     <t>CanBeModified</t>
   </si>
   <si>
-    <t>StatusEffects</t>
-  </si>
-  <si>
     <t>Consumable</t>
   </si>
   <si>
@@ -118,21 +116,9 @@
     <t>False</t>
   </si>
   <si>
-    <t>Enemy</t>
-  </si>
-  <si>
-    <t>Ally</t>
-  </si>
-  <si>
     <t>All</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
-    <t>Others</t>
-  </si>
-  <si>
     <t>Line</t>
   </si>
   <si>
@@ -211,9 +197,6 @@
     <t>PushFix_3</t>
   </si>
   <si>
-    <t>TeleportTo</t>
-  </si>
-  <si>
     <t>FloorStatus</t>
   </si>
   <si>
@@ -242,6 +225,69 @@
   </si>
   <si>
     <t>None</t>
+  </si>
+  <si>
+    <t>Square</t>
+  </si>
+  <si>
+    <t>Perpendicular</t>
+  </si>
+  <si>
+    <t>OnlyAlly</t>
+  </si>
+  <si>
+    <t>OnlyEnemy</t>
+  </si>
+  <si>
+    <t>OnlySelf</t>
+  </si>
+  <si>
+    <t>OnlyOthers</t>
+  </si>
+  <si>
+    <t>OnlyUnits</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Assassinskill_46</t>
+  </si>
+  <si>
+    <t>Poison Cocktail</t>
+  </si>
+  <si>
+    <t>Tentacule</t>
+  </si>
+  <si>
+    <t>Shamanskill_33</t>
+  </si>
+  <si>
+    <t>healing</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Shamanskill_12</t>
+  </si>
+  <si>
+    <t>Leef Razor</t>
+  </si>
+  <si>
+    <t>Wind Arrow</t>
+  </si>
+  <si>
+    <t>Warriorskill_17</t>
+  </si>
+  <si>
+    <t>Assassinskill_40</t>
+  </si>
+  <si>
+    <t>Discharge Hit</t>
+  </si>
+  <si>
+    <t>Teleport_to</t>
   </si>
 </sst>
 </file>
@@ -559,32 +605,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="4.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
@@ -592,28 +640,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="C1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="H1" t="s">
         <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -640,16 +688,16 @@
         <v>9</v>
       </c>
       <c r="R1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="S1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="T1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -657,52 +705,52 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D2">
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K2">
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O2" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" t="s">
         <v>26</v>
       </c>
-      <c r="P2" t="s">
-        <v>29</v>
-      </c>
       <c r="Q2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R2">
         <v>5</v>
       </c>
       <c r="S2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T2" t="s">
+        <v>54</v>
+      </c>
+      <c r="U2" t="s">
         <v>60</v>
-      </c>
-      <c r="U2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -710,52 +758,52 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <v>3</v>
       </c>
       <c r="L3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="Q3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="T3" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="U3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -763,55 +811,385 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
-        <v>68</v>
-      </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="O4" t="s">
+        <v>25</v>
+      </c>
+      <c r="P4" t="s">
         <v>26</v>
       </c>
-      <c r="P4" t="s">
-        <v>29</v>
-      </c>
       <c r="Q4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="R4">
+        <v>5</v>
+      </c>
+      <c r="S4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T4" t="s">
+        <v>57</v>
+      </c>
+      <c r="U4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>3</v>
       </c>
-      <c r="S4" t="s">
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5" t="s">
+        <v>16</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P5" t="s">
         <v>26</v>
       </c>
-      <c r="T4" t="s">
-        <v>63</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+      <c r="R5">
+        <v>3</v>
+      </c>
+      <c r="S5" t="s">
+        <v>25</v>
+      </c>
+      <c r="T5" t="s">
+        <v>71</v>
+      </c>
+      <c r="U5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" t="s">
+        <v>42</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>16</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" t="s">
+        <v>25</v>
+      </c>
+      <c r="P6" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6">
+        <v>3</v>
+      </c>
+      <c r="S6" t="s">
+        <v>25</v>
+      </c>
+      <c r="T6" t="s">
+        <v>74</v>
+      </c>
+      <c r="U6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7">
+        <v>3</v>
+      </c>
+      <c r="L7" t="s">
+        <v>64</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" t="s">
+        <v>25</v>
+      </c>
+      <c r="P7" t="s">
         <v>66</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7" t="s">
+        <v>25</v>
+      </c>
+      <c r="T7" t="s">
+        <v>75</v>
+      </c>
+      <c r="U7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8">
+        <v>2</v>
+      </c>
+      <c r="N8" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" t="s">
+        <v>25</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>24</v>
+      </c>
+      <c r="R8">
+        <v>3</v>
+      </c>
+      <c r="S8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T8" t="s">
+        <v>77</v>
+      </c>
+      <c r="U8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O9" t="s">
+        <v>25</v>
+      </c>
+      <c r="P9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9">
+        <v>6</v>
+      </c>
+      <c r="S9" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9" t="s">
+        <v>80</v>
+      </c>
+      <c r="U9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
+        <v>64</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10" t="s">
+        <v>24</v>
+      </c>
+      <c r="O10" t="s">
+        <v>25</v>
+      </c>
+      <c r="P10" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>24</v>
+      </c>
+      <c r="R10">
+        <v>5</v>
+      </c>
+      <c r="S10" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" t="s">
+        <v>81</v>
+      </c>
+      <c r="U10" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -835,7 +1213,7 @@
           </x14:formula1>
           <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{F7EBE28F-E1ED-4A6A-8276-74ADCD55510B}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F7EBE28F-E1ED-4A6A-8276-74ADCD55510B}">
           <x14:formula1>
             <xm:f>Enum!$C$2:$C$5</xm:f>
           </x14:formula1>
@@ -859,9 +1237,21 @@
           </x14:formula1>
           <xm:sqref>P2:P1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B48493F7-4EB2-4A53-9A24-CF4F42CFF5FA}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A142BD8C-C3F8-44CC-8AC6-94BB65A34F74}">
           <x14:formula1>
-            <xm:f>Enum!$F$2:$F$352</xm:f>
+            <xm:f>Enum!$I$1</xm:f>
+          </x14:formula1>
+          <xm:sqref>U1:U1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{42AF8CDE-0350-4655-A006-BBEA1F8A2C14}">
+          <x14:formula1>
+            <xm:f>Enum!$H$3:$H$44</xm:f>
+          </x14:formula1>
+          <xm:sqref>I2:I1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{813F82CD-8383-483B-AC51-C1F98364FAE3}">
+          <x14:formula1>
+            <xm:f>Enum!$F$2:$F$53</xm:f>
           </x14:formula1>
           <xm:sqref>E2:G1048576</xm:sqref>
         </x14:dataValidation>
@@ -871,18 +1261,6 @@
           </x14:formula1>
           <xm:sqref>H2:H1048576</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{42AF8CDE-0350-4655-A006-BBEA1F8A2C14}">
-          <x14:formula1>
-            <xm:f>Enum!$H$2:$H$44</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{A142BD8C-C3F8-44CC-8AC6-94BB65A34F74}">
-          <x14:formula1>
-            <xm:f>Enum!$I$1</xm:f>
-          </x14:formula1>
-          <xm:sqref>U1:U1048576</xm:sqref>
-        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -891,71 +1269,72 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E04AA25F-47DC-4AD0-8D6C-77D50FE882A2}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="G1" t="s">
         <v>1</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="I1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="H2" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -966,118 +1345,132 @@
         <v>16</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="H3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="F4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" t="s">
+        <v>83</v>
+      </c>
+      <c r="H4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
         <v>42</v>
       </c>
-      <c r="G4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" t="s">
-        <v>43</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
-      </c>
       <c r="H5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="F6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="F9" t="s">
-        <v>59</v>
-      </c>
       <c r="H9" t="s">
-        <v>56</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>